<commit_message>
add to negative test case
</commit_message>
<xml_diff>
--- a/databiding.xlsx
+++ b/databiding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="4" r:id="rId1"/>
@@ -114,10 +114,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -136,14 +136,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -151,52 +174,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -211,38 +196,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -258,6 +214,50 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -294,187 +294,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,13 +503,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,7 +537,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -542,22 +557,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,148 +605,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1094,14 +1094,14 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="2" width="9.66666666666667" customWidth="1"/>
     <col min="3" max="3" width="12.7777777777778" customWidth="1"/>
-    <col min="4" max="4" width="12.5555555555556" customWidth="1"/>
+    <col min="4" max="4" width="14.2222222222222" customWidth="1"/>
     <col min="5" max="5" width="7.77777777777778" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1150,8 +1150,8 @@
   <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F17:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
@@ -1217,7 +1217,7 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test case negative CBS_MASS_ACCOUNT_1.3
</commit_message>
<xml_diff>
--- a/databiding.xlsx
+++ b/databiding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9024"/>
+    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>username</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>pilih1</t>
+  </si>
+  <si>
+    <t>00005</t>
+  </si>
+  <si>
+    <t>00069</t>
+  </si>
+  <si>
+    <t>00070</t>
   </si>
   <si>
     <t>pilihDetail</t>
@@ -118,8 +127,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
@@ -139,31 +148,77 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,98 +233,52 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,31 +306,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,43 +444,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,78 +474,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -466,12 +481,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,28 +515,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,26 +548,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -589,17 +587,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -608,15 +617,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -626,130 +635,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1096,7 +1105,7 @@
   <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1151,13 +1160,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="25.8888888888889" customWidth="1"/>
     <col min="2" max="2" width="22.4444444444444" customWidth="1"/>
@@ -1206,9 +1215,72 @@
         <v>21</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://172.31.1.93:9000/"/>
+    <hyperlink ref="A3" r:id="rId1" display="http://172.31.1.93:9000/"/>
+    <hyperlink ref="A4" r:id="rId1" display="http://172.31.1.93:9000/" tooltip="http://172.31.1.93:9000/"/>
+    <hyperlink ref="A5" r:id="rId1" display="http://172.31.1.93:9000/" tooltip="http://172.31.1.93:9000/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1240,10 +1312,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:4">
@@ -1254,10 +1326,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1291,10 +1363,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:4">
@@ -1305,7 +1377,7 @@
         <v>33333333</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2">
         <v>44707</v>
@@ -1319,10 +1391,10 @@
         <v>33333333</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="5:5">

</xml_diff>

<commit_message>
Negative case mass opening
</commit_message>
<xml_diff>
--- a/databiding.xlsx
+++ b/databiding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9024" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>username</t>
   </si>
@@ -94,6 +94,9 @@
     <t>00070</t>
   </si>
   <si>
+    <t>00071</t>
+  </si>
+  <si>
     <t>pilihDetail</t>
   </si>
   <si>
@@ -106,16 +109,10 @@
     <t>accept</t>
   </si>
   <si>
-    <t>cases</t>
-  </si>
-  <si>
     <t>tanggal</t>
   </si>
   <si>
-    <t>positive1</t>
-  </si>
-  <si>
-    <t>negative1</t>
+    <t>25/05/2022</t>
   </si>
   <si>
     <t>121212133434</t>
@@ -126,9 +123,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
@@ -154,11 +151,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -169,25 +165,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,10 +188,65 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -216,76 +258,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -306,55 +303,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,72 +477,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -439,54 +484,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,23 +515,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -563,26 +545,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,6 +577,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -617,158 +614,161 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -782,6 +782,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1118,36 +1121,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1160,13 +1163,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="25.8888888888889" customWidth="1"/>
     <col min="2" max="2" width="22.4444444444444" customWidth="1"/>
@@ -1175,103 +1178,123 @@
     <col min="5" max="5" width="15.1111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="2" customFormat="1" spans="1:6">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:6">
-      <c r="A2" s="5" t="s">
+    <row r="2" s="2" customFormat="1" spans="1:6">
+      <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1281,6 +1304,7 @@
     <hyperlink ref="A3" r:id="rId1" display="http://172.31.1.93:9000/"/>
     <hyperlink ref="A4" r:id="rId1" display="http://172.31.1.93:9000/" tooltip="http://172.31.1.93:9000/"/>
     <hyperlink ref="A5" r:id="rId1" display="http://172.31.1.93:9000/" tooltip="http://172.31.1.93:9000/"/>
+    <hyperlink ref="A6" r:id="rId1" display="http://172.31.1.93:9000/" tooltip="http://172.31.1.93:9000/"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1305,31 +1329,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="D1" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:4">
-      <c r="A2" s="6" t="s">
+    <row r="2" s="2" customFormat="1" spans="1:4">
+      <c r="A2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1341,64 +1365,31 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="12.8888888888889" customWidth="1"/>
-    <col min="2" max="2" width="17.3333333333333" customWidth="1"/>
-    <col min="3" max="3" width="21.6666666666667" customWidth="1"/>
-    <col min="4" max="4" width="16.8888888888889" customWidth="1"/>
+    <col min="1" max="1" width="16.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:1">
+      <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:4">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1">
-        <v>33333333</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="2" s="2" customFormat="1" spans="1:1">
+      <c r="A2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="2">
-        <v>44707</v>
-      </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>33333333</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="5:5">
-      <c r="E6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>